<commit_message>
Added self calibration to FontBaseExtensions width calculator
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Misc/AdjustToContents.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Misc/AdjustToContents.xlsx
@@ -3563,24 +3563,24 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="4.570625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="50.600625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="70.174584" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="69.617876" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="68.694739" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="67.412197" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="65.780013" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="63.810607" style="0" customWidth="1"/>
-    <x:col min="9" max="9" width="61.518968" style="0" customWidth="1"/>
-    <x:col min="10" max="10" width="58.922538" style="0" customWidth="1"/>
-    <x:col min="11" max="11" width="56.041076" style="0" customWidth="1"/>
-    <x:col min="12" max="12" width="52.896511" style="0" customWidth="1"/>
-    <x:col min="13" max="13" width="49.512777" style="0" customWidth="1"/>
-    <x:col min="14" max="14" width="45.915625" style="0" customWidth="1"/>
-    <x:col min="15" max="15" width="42.132432" style="0" customWidth="1"/>
-    <x:col min="16" max="16" width="38.19199" style="0" customWidth="1"/>
-    <x:col min="17" max="17" width="34.124288" style="0" customWidth="1"/>
-    <x:col min="18" max="18" width="29.960284" style="0" customWidth="1"/>
-    <x:col min="19" max="19" width="25.731669" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="50.590625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="70.164622" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="69.608028" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="68.685079" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="67.4028" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="65.77095" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="63.801947" style="0" customWidth="1"/>
+    <x:col min="9" max="9" width="61.510777" style="0" customWidth="1"/>
+    <x:col min="10" max="10" width="58.914877" style="0" customWidth="1"/>
+    <x:col min="11" max="11" width="56.034004" style="0" customWidth="1"/>
+    <x:col min="12" max="12" width="52.890083" style="0" customWidth="1"/>
+    <x:col min="13" max="13" width="49.507041" style="0" customWidth="1"/>
+    <x:col min="14" max="14" width="45.910625" style="0" customWidth="1"/>
+    <x:col min="15" max="15" width="42.128206" style="0" customWidth="1"/>
+    <x:col min="16" max="16" width="38.18857" style="0" customWidth="1"/>
+    <x:col min="17" max="17" width="34.1217" style="0" customWidth="1"/>
+    <x:col min="18" max="18" width="29.958548" style="0" customWidth="1"/>
+    <x:col min="19" max="19" width="25.730798" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:19">

</xml_diff>

<commit_message>
Rows with changes height shouldn't indicate that they also have a custom row style when the style is not specified. In case of a row with same style as worksheet but custom height, the missing row style is not displayed as a a worksheet style.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Misc/AdjustToContents.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Misc/AdjustToContents.xlsx
@@ -3404,12 +3404,12 @@
     <x:col min="2" max="2" width="28.190625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:2" customFormat="1" ht="41.5039" customHeight="1">
+    <x:row r="1" spans="1:2" ht="41.5039" customHeight="1">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:2" customFormat="1" ht="27.669267" customHeight="1">
+    <x:row r="2" spans="1:2" ht="27.669267" customHeight="1">
       <x:c r="A2" s="2" t="s">
         <x:v>1</x:v>
       </x:c>
@@ -3662,97 +3662,97 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:1" customFormat="1" ht="304.361925" customHeight="1">
+    <x:row r="1" spans="1:1" ht="304.361925" customHeight="1">
       <x:c r="A1" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:1" customFormat="1" ht="15.218096" customHeight="1">
+    <x:row r="2" spans="1:1" ht="15.218096" customHeight="1">
       <x:c r="A2" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:1" customFormat="1" ht="7.609048" customHeight="1">
+    <x:row r="3" spans="1:1" ht="7.609048" customHeight="1">
       <x:c r="A3" s="4" t="s">
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:1" customFormat="1" ht="16.063546" customHeight="1">
+    <x:row r="4" spans="1:1" ht="16.063546" customHeight="1">
       <x:c r="A4" s="5" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:1" customFormat="1" ht="24.095319" customHeight="1">
+    <x:row r="5" spans="1:1" ht="24.095319" customHeight="1">
       <x:c r="A5" s="6" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:1" customFormat="1" ht="32.127092" customHeight="1">
+    <x:row r="6" spans="1:1" ht="32.127092" customHeight="1">
       <x:c r="A6" s="7" t="s">
         <x:v>11</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:1" customFormat="1" ht="40.158865" customHeight="1">
+    <x:row r="7" spans="1:1" ht="40.158865" customHeight="1">
       <x:c r="A7" s="8" t="s">
         <x:v>12</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:1" customFormat="1" ht="48.190638" customHeight="1">
+    <x:row r="8" spans="1:1" ht="48.190638" customHeight="1">
       <x:c r="A8" s="9" t="s">
         <x:v>13</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:1" customFormat="1" ht="56.222411" customHeight="1">
+    <x:row r="9" spans="1:1" ht="56.222411" customHeight="1">
       <x:c r="A9" s="10" t="s">
         <x:v>14</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:1" customFormat="1" ht="64.254184" customHeight="1">
+    <x:row r="10" spans="1:1" ht="64.254184" customHeight="1">
       <x:c r="A10" s="11" t="s">
         <x:v>15</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:1" customFormat="1" ht="72.285957" customHeight="1">
+    <x:row r="11" spans="1:1" ht="72.285957" customHeight="1">
       <x:c r="A11" s="12" t="s">
         <x:v>16</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:1" customFormat="1" ht="80.31773" customHeight="1">
+    <x:row r="12" spans="1:1" ht="80.31773" customHeight="1">
       <x:c r="A12" s="13" t="s">
         <x:v>17</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:1" customFormat="1" ht="88.349503" customHeight="1">
+    <x:row r="13" spans="1:1" ht="88.349503" customHeight="1">
       <x:c r="A13" s="14" t="s">
         <x:v>18</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:1" customFormat="1" ht="96.381276" customHeight="1">
+    <x:row r="14" spans="1:1" ht="96.381276" customHeight="1">
       <x:c r="A14" s="15" t="s">
         <x:v>19</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:1" customFormat="1" ht="104.413049" customHeight="1">
+    <x:row r="15" spans="1:1" ht="104.413049" customHeight="1">
       <x:c r="A15" s="16" t="s">
         <x:v>20</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:1" customFormat="1" ht="112.444822" customHeight="1">
+    <x:row r="16" spans="1:1" ht="112.444822" customHeight="1">
       <x:c r="A16" s="17" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:1" customFormat="1" ht="120.476595" customHeight="1">
+    <x:row r="17" spans="1:1" ht="120.476595" customHeight="1">
       <x:c r="A17" s="18" t="s">
         <x:v>22</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:1" customFormat="1" ht="128.508368" customHeight="1">
+    <x:row r="18" spans="1:1" ht="128.508368" customHeight="1">
       <x:c r="A18" s="19" t="s">
         <x:v>23</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:1" customFormat="1" ht="136.540141" customHeight="1">
+    <x:row r="19" spans="1:1" ht="136.540141" customHeight="1">
       <x:c r="A19" s="20" t="s">
         <x:v>24</x:v>
       </x:c>
@@ -3777,97 +3777,97 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:1" customFormat="1" ht="304.361925" customHeight="1">
+    <x:row r="1" spans="1:1" ht="304.361925" customHeight="1">
       <x:c r="A1" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:1" customFormat="1" ht="83.0078" customHeight="1">
+    <x:row r="2" spans="1:1" ht="83.0078" customHeight="1">
       <x:c r="A2" s="0" t="s">
         <x:v>43</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:1" customFormat="1" ht="17.293292" customHeight="1">
+    <x:row r="3" spans="1:1" ht="17.293292" customHeight="1">
       <x:c r="A3" s="4" t="s">
         <x:v>44</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:1" customFormat="1" ht="34.586583" customHeight="1">
+    <x:row r="4" spans="1:1" ht="34.586583" customHeight="1">
       <x:c r="A4" s="5" t="s">
         <x:v>45</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:1" customFormat="1" ht="51.879875" customHeight="1">
+    <x:row r="5" spans="1:1" ht="51.879875" customHeight="1">
       <x:c r="A5" s="6" t="s">
         <x:v>46</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:1" customFormat="1" ht="69.173166" customHeight="1">
+    <x:row r="6" spans="1:1" ht="69.173166" customHeight="1">
       <x:c r="A6" s="7" t="s">
         <x:v>47</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:1" customFormat="1" ht="86.466458" customHeight="1">
+    <x:row r="7" spans="1:1" ht="86.466458" customHeight="1">
       <x:c r="A7" s="8" t="s">
         <x:v>48</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:1" customFormat="1" ht="103.759749" customHeight="1">
+    <x:row r="8" spans="1:1" ht="103.759749" customHeight="1">
       <x:c r="A8" s="9" t="s">
         <x:v>49</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:1" customFormat="1" ht="121.053041" customHeight="1">
+    <x:row r="9" spans="1:1" ht="121.053041" customHeight="1">
       <x:c r="A9" s="10" t="s">
         <x:v>50</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:1" customFormat="1" ht="138.346333" customHeight="1">
+    <x:row r="10" spans="1:1" ht="138.346333" customHeight="1">
       <x:c r="A10" s="11" t="s">
         <x:v>51</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:1" customFormat="1" ht="155.639624" customHeight="1">
+    <x:row r="11" spans="1:1" ht="155.639624" customHeight="1">
       <x:c r="A11" s="12" t="s">
         <x:v>52</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:1" customFormat="1" ht="172.932916" customHeight="1">
+    <x:row r="12" spans="1:1" ht="172.932916" customHeight="1">
       <x:c r="A12" s="13" t="s">
         <x:v>53</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:1" customFormat="1" ht="190.226207" customHeight="1">
+    <x:row r="13" spans="1:1" ht="190.226207" customHeight="1">
       <x:c r="A13" s="14" t="s">
         <x:v>54</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:1" customFormat="1" ht="207.519499" customHeight="1">
+    <x:row r="14" spans="1:1" ht="207.519499" customHeight="1">
       <x:c r="A14" s="15" t="s">
         <x:v>55</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:1" customFormat="1" ht="224.81279" customHeight="1">
+    <x:row r="15" spans="1:1" ht="224.81279" customHeight="1">
       <x:c r="A15" s="16" t="s">
         <x:v>56</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:1" customFormat="1" ht="242.106082" customHeight="1">
+    <x:row r="16" spans="1:1" ht="242.106082" customHeight="1">
       <x:c r="A16" s="17" t="s">
         <x:v>57</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:1" customFormat="1" ht="259.399374" customHeight="1">
+    <x:row r="17" spans="1:1" ht="259.399374" customHeight="1">
       <x:c r="A17" s="18" t="s">
         <x:v>58</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:1" customFormat="1" ht="276.692665" customHeight="1">
+    <x:row r="18" spans="1:1" ht="276.692665" customHeight="1">
       <x:c r="A18" s="19" t="s">
         <x:v>59</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:1" customFormat="1" ht="293.985957" customHeight="1">
+    <x:row r="19" spans="1:1" ht="293.985957" customHeight="1">
       <x:c r="A19" s="20" t="s">
         <x:v>60</x:v>
       </x:c>

</xml_diff>

<commit_message>
Reverted attempt to cope with openxmlsdk behavior that causes rounding diff between .net and .net legacy
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Misc/AdjustToContents.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Misc/AdjustToContents.xlsx
@@ -3465,17 +3465,17 @@
     <x:col min="1" max="1" width="4.505971" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="17.166487" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="19.721622" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="20.72679" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="20.726789" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="20.239899" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="19.983696" style="0" customWidth="1"/>
     <x:col min="7" max="7" width="19.268783" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="18.77032" style="0" customWidth="1"/>
-    <x:col min="9" max="9" width="17.849107" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="18.770319" style="0" customWidth="1"/>
+    <x:col min="9" max="9" width="17.849106" style="0" customWidth="1"/>
     <x:col min="10" max="10" width="17.123528" style="0" customWidth="1"/>
-    <x:col min="11" max="11" width="16.024006" style="0" customWidth="1"/>
-    <x:col min="12" max="12" width="15.093359" style="0" customWidth="1"/>
+    <x:col min="11" max="11" width="16.024005" style="0" customWidth="1"/>
+    <x:col min="12" max="12" width="15.093358" style="0" customWidth="1"/>
     <x:col min="13" max="13" width="13.848935" style="0" customWidth="1"/>
-    <x:col min="14" max="14" width="12.741497" style="0" customWidth="1"/>
+    <x:col min="14" max="14" width="12.741496" style="0" customWidth="1"/>
     <x:col min="15" max="15" width="11.389983" style="0" customWidth="1"/>
     <x:col min="16" max="16" width="10.139402" style="0" customWidth="1"/>
     <x:col min="17" max="17" width="8.721864" style="0" customWidth="1"/>
@@ -3578,9 +3578,9 @@
     <x:col min="14" max="14" width="44.995425" style="0" customWidth="1"/>
     <x:col min="15" max="15" width="41.292112" style="0" customWidth="1"/>
     <x:col min="16" max="16" width="37.434871" style="0" customWidth="1"/>
-    <x:col min="17" max="17" width="33.453057" style="0" customWidth="1"/>
-    <x:col min="18" max="18" width="29.376974" style="0" customWidth="1"/>
-    <x:col min="19" max="19" width="25.237644" style="0" customWidth="1"/>
+    <x:col min="17" max="17" width="33.453056" style="0" customWidth="1"/>
+    <x:col min="18" max="18" width="29.376973" style="0" customWidth="1"/>
+    <x:col min="19" max="19" width="25.237643" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:19">

</xml_diff>